<commit_message>
Saving players, viewing coolness
</commit_message>
<xml_diff>
--- a/lib/tasks/de.xlsx
+++ b/lib/tasks/de.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>Rank</t>
   </si>
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t>Team</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
   <si>
     <t>Florida State</t>
@@ -123,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -135,12 +138,17 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
@@ -153,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -176,27 +184,150 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1447,7 +1578,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1456,8 +1587,10 @@
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6797" style="1" customWidth="1"/>
-    <col min="5" max="256" width="6" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6" style="1" customWidth="1"/>
+    <col min="7" max="256" width="6" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
@@ -1473,365 +1606,551 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="3">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" ht="17" customHeight="1">
-      <c r="A2" s="3">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" s="6"/>
+      <c r="C2" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" ht="17" customHeight="1">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" ht="17" customHeight="1">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="E4" s="7">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" ht="17" customHeight="1">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" t="s" s="2">
+      <c r="B5" s="9"/>
+      <c r="C5" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" ht="17" customHeight="1">
-      <c r="A3" s="3">
+      <c r="F5" s="8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" ht="17" customHeight="1">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E6" s="7">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" ht="17" customHeight="1">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7">
+        <v>6</v>
+      </c>
+      <c r="F7" s="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" ht="17" customHeight="1">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="E8" s="7">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" ht="17" customHeight="1">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7">
+        <v>8</v>
+      </c>
+      <c r="F9" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" ht="17" customHeight="1">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="E10" s="7">
+        <v>9</v>
+      </c>
+      <c r="F10" s="8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" ht="17" customHeight="1">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E11" s="7">
+        <v>10</v>
+      </c>
+      <c r="F11" s="8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" ht="17" customHeight="1">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="E12" s="7">
+        <v>11</v>
+      </c>
+      <c r="F12" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" ht="17" customHeight="1">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="E13" s="7">
+        <v>12</v>
+      </c>
+      <c r="F13" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" ht="17" customHeight="1">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="E14" s="7">
+        <v>13</v>
+      </c>
+      <c r="F14" s="8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" ht="17" customHeight="1">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="E15" s="7">
+        <v>14</v>
+      </c>
+      <c r="F15" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" ht="17" customHeight="1">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="E16" s="7">
+        <v>15</v>
+      </c>
+      <c r="F16" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" ht="17" customHeight="1">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="E17" s="7">
+        <v>16</v>
+      </c>
+      <c r="F17" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" ht="17" customHeight="1">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="E18" s="7">
+        <v>17</v>
+      </c>
+      <c r="F18" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" ht="17" customHeight="1">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="E19" s="7">
+        <v>18</v>
+      </c>
+      <c r="F19" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" ht="17" customHeight="1">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="E20" s="7">
+        <v>19</v>
+      </c>
+      <c r="F20" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" ht="17" customHeight="1">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="E21" s="7">
+        <v>20</v>
+      </c>
+      <c r="F21" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" ht="17" customHeight="1">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="E22" s="7">
+        <v>21</v>
+      </c>
+      <c r="F22" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" ht="17" customHeight="1">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="E23" s="7">
+        <v>22</v>
+      </c>
+      <c r="F23" s="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" ht="17" customHeight="1">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="E24" s="7">
+        <v>23</v>
+      </c>
+      <c r="F24" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" ht="17" customHeight="1">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="E25" s="7">
+        <v>24</v>
+      </c>
+      <c r="F25" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" ht="17" customHeight="1">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="D26" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="E26" s="7">
+        <v>25</v>
+      </c>
+      <c r="F26" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" ht="17" customHeight="1">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="E27" s="7">
+        <v>26</v>
+      </c>
+      <c r="F27" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" ht="17" customHeight="1">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="E28" s="7">
+        <v>27</v>
+      </c>
+      <c r="F28" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" ht="17" customHeight="1">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D29" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="E29" s="7">
+        <v>28</v>
+      </c>
+      <c r="F29" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" ht="17" customHeight="1">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="E30" s="7">
+        <v>29</v>
+      </c>
+      <c r="F30" s="8">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" t="s" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" ht="17" customHeight="1">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" t="s" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" ht="17" customHeight="1">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" t="s" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" ht="17" customHeight="1">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" t="s" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" ht="17" customHeight="1">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" t="s" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" ht="17" customHeight="1">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" t="s" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" ht="17" customHeight="1">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" t="s" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" ht="17" customHeight="1">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" t="s" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" ht="17" customHeight="1">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" t="s" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" ht="17" customHeight="1">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" t="s" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" ht="17" customHeight="1">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" t="s" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" ht="17" customHeight="1">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" t="s" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" ht="17" customHeight="1">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" t="s" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" ht="17" customHeight="1">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" t="s" s="2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" ht="17" customHeight="1">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" t="s" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" ht="17" customHeight="1">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" ht="17" customHeight="1">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" t="s" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" ht="17" customHeight="1">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" t="s" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" ht="17" customHeight="1">
-      <c r="A21" s="3">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" t="s" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" ht="17" customHeight="1">
-      <c r="A22" s="3">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" t="s" s="2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" ht="17" customHeight="1">
-      <c r="A23" s="3">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" t="s" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" ht="17" customHeight="1">
-      <c r="A24" s="3">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" t="s" s="2">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" ht="17" customHeight="1">
-      <c r="A25" s="3">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" t="s" s="2">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" ht="17" customHeight="1">
-      <c r="A26" s="3">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" t="s" s="2">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" ht="17" customHeight="1">
-      <c r="A27" s="3">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" t="s" s="2">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" ht="17" customHeight="1">
-      <c r="A28" s="3">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s" s="2">
+    </row>
+    <row r="31" ht="17" customHeight="1">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" t="s" s="2">
+      <c r="B31" s="10"/>
+      <c r="C31" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="E31" s="11">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" ht="17" customHeight="1">
-      <c r="A29" s="3">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" t="s" s="2">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" ht="17" customHeight="1">
-      <c r="A30" s="3">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" ht="17" customHeight="1">
-      <c r="A31" s="3">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" t="s" s="2">
-        <v>33</v>
+      <c r="F31" s="12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>